<commit_message>
fix: improve presentation of Project Euler 11
</commit_message>
<xml_diff>
--- a/Project Euler 011.xlsx
+++ b/Project Euler 011.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A936D32-A463-45CE-8786-D606F5723B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6437FA1C-4B03-4F2F-979A-A32798B7A507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +204,14 @@
     <font>
       <b/>
       <sz val="28"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -557,7 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -567,6 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2202,7 +2211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41A5A53-CD55-4276-A79C-83D8922F3FC4}">
   <dimension ref="B5:AQ64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -8585,8 +8594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D608A6F-8481-498F-959A-C5D3AB51DD5E}">
   <dimension ref="B2:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8595,8 +8604,8 @@
     <col min="4" max="23" width="3.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:23" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: improve Project Euler 11
</commit_message>
<xml_diff>
--- a/Project Euler 011.xlsx
+++ b/Project Euler 011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7ACFB1-86A4-403C-A384-3AA145905865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AB139B-2167-46C4-B820-2481DE5C5FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="question and data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>&lt;-- answer</t>
   </si>
@@ -54,6 +54,9 @@
   <si>
     <t>in the 20 x 20 grid?</t>
   </si>
+  <si>
+    <t>https://projecteuler.net/problem=11</t>
+  </si>
 </sst>
 </file>
 
@@ -62,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +242,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,7 +566,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -590,8 +609,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -602,53 +622,55 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,7 +686,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -980,13 +1002,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:U28"/>
+  <dimension ref="B2:U29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="21" width="3.90625" customWidth="1"/>
   </cols>
@@ -1000,1139 +1022,1082 @@
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B7" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B9" s="6">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>22</v>
-      </c>
-      <c r="E9" s="6">
-        <v>97</v>
-      </c>
-      <c r="F9" s="6">
-        <v>38</v>
-      </c>
-      <c r="G9" s="6">
-        <v>15</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>40</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>75</v>
-      </c>
-      <c r="L9" s="6">
-        <v>4</v>
-      </c>
-      <c r="M9" s="6">
-        <v>5</v>
-      </c>
-      <c r="N9" s="6">
-        <v>7</v>
-      </c>
-      <c r="O9" s="6">
-        <v>78</v>
-      </c>
-      <c r="P9" s="6">
-        <v>52</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>12</v>
-      </c>
-      <c r="R9" s="6">
-        <v>50</v>
-      </c>
-      <c r="S9" s="6">
-        <v>77</v>
-      </c>
-      <c r="T9" s="6">
-        <v>91</v>
-      </c>
-      <c r="U9" s="6">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="D10" s="6">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="E10" s="6">
+        <v>97</v>
+      </c>
+      <c r="F10" s="6">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
         <v>40</v>
       </c>
-      <c r="F10" s="6">
-        <v>17</v>
-      </c>
-      <c r="G10" s="6">
-        <v>81</v>
-      </c>
-      <c r="H10" s="6">
-        <v>18</v>
-      </c>
-      <c r="I10" s="6">
-        <v>57</v>
-      </c>
       <c r="J10" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K10" s="6">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="L10" s="6">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="M10" s="6">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="N10" s="6">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="O10" s="6">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="P10" s="6">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="Q10" s="6">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="R10" s="6">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="S10" s="6">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="T10" s="6">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="U10" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6">
         <v>49</v>
       </c>
       <c r="D11" s="6">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="E11" s="6">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="F11" s="6">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G11" s="6">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H11" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I11" s="6">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J11" s="6">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="K11" s="6">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="L11" s="6">
+        <v>17</v>
+      </c>
+      <c r="M11" s="6">
         <v>40</v>
       </c>
-      <c r="M11" s="6">
-        <v>67</v>
-      </c>
       <c r="N11" s="6">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O11" s="6">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="P11" s="6">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="6">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="R11" s="6">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="S11" s="6">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="T11" s="6">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="U11" s="6">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="C12" s="6">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D12" s="6">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F12" s="6">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="G12" s="6">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="H12" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I12" s="6">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J12" s="6">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="K12" s="6">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="L12" s="6">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="M12" s="6">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="N12" s="6">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="O12" s="6">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="P12" s="6">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="6">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="R12" s="6">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="S12" s="6">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="T12" s="6">
         <v>36</v>
       </c>
       <c r="U12" s="6">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C13" s="6">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="E13" s="6">
+        <v>23</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
+      <c r="G13" s="6">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6">
+        <v>42</v>
+      </c>
+      <c r="J13" s="6">
+        <v>69</v>
+      </c>
+      <c r="K13" s="6">
+        <v>24</v>
+      </c>
+      <c r="L13" s="6">
+        <v>68</v>
+      </c>
+      <c r="M13" s="6">
+        <v>56</v>
+      </c>
+      <c r="N13" s="6">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
+        <v>32</v>
+      </c>
+      <c r="P13" s="6">
+        <v>56</v>
+      </c>
+      <c r="Q13" s="6">
         <v>71</v>
       </c>
-      <c r="F13" s="6">
-        <v>51</v>
-      </c>
-      <c r="G13" s="6">
-        <v>67</v>
-      </c>
-      <c r="H13" s="6">
-        <v>63</v>
-      </c>
-      <c r="I13" s="6">
-        <v>89</v>
-      </c>
-      <c r="J13" s="6">
-        <v>41</v>
-      </c>
-      <c r="K13" s="6">
-        <v>92</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="R13" s="6">
+        <v>37</v>
+      </c>
+      <c r="S13" s="6">
+        <v>2</v>
+      </c>
+      <c r="T13" s="6">
         <v>36</v>
       </c>
-      <c r="M13" s="6">
-        <v>54</v>
-      </c>
-      <c r="N13" s="6">
-        <v>22</v>
-      </c>
-      <c r="O13" s="6">
-        <v>40</v>
-      </c>
-      <c r="P13" s="6">
-        <v>40</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>28</v>
-      </c>
-      <c r="R13" s="6">
-        <v>66</v>
-      </c>
-      <c r="S13" s="6">
-        <v>33</v>
-      </c>
-      <c r="T13" s="6">
-        <v>13</v>
-      </c>
       <c r="U13" s="6">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F14" s="6">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="G14" s="6">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="H14" s="6">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="I14" s="6">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="J14" s="6">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K14" s="6">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="L14" s="6">
+        <v>36</v>
+      </c>
+      <c r="M14" s="6">
+        <v>54</v>
+      </c>
+      <c r="N14" s="6">
+        <v>22</v>
+      </c>
+      <c r="O14" s="6">
+        <v>40</v>
+      </c>
+      <c r="P14" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>28</v>
+      </c>
+      <c r="R14" s="6">
+        <v>66</v>
+      </c>
+      <c r="S14" s="6">
         <v>33</v>
       </c>
-      <c r="M14" s="6">
-        <v>53</v>
-      </c>
-      <c r="N14" s="6">
-        <v>78</v>
-      </c>
-      <c r="O14" s="6">
-        <v>36</v>
-      </c>
-      <c r="P14" s="6">
-        <v>84</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>20</v>
-      </c>
-      <c r="R14" s="6">
-        <v>35</v>
-      </c>
-      <c r="S14" s="6">
-        <v>17</v>
-      </c>
       <c r="T14" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U14" s="6">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6">
+        <v>47</v>
+      </c>
+      <c r="D15" s="6">
         <v>32</v>
       </c>
-      <c r="C15" s="6">
-        <v>98</v>
-      </c>
-      <c r="D15" s="6">
-        <v>81</v>
-      </c>
       <c r="E15" s="6">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F15" s="6">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="G15" s="6">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="H15" s="6">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I15" s="6">
-        <v>10</v>
-      </c>
-      <c r="J15" s="11">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="J15" s="6">
+        <v>44</v>
       </c>
       <c r="K15" s="6">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="L15" s="6">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="M15" s="6">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="N15" s="6">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="O15" s="6">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="P15" s="6">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="6">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="R15" s="6">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="S15" s="6">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="T15" s="6">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="U15" s="6">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6">
+        <v>98</v>
+      </c>
+      <c r="D16" s="6">
+        <v>81</v>
+      </c>
+      <c r="E16" s="6">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6">
+        <v>64</v>
+      </c>
+      <c r="G16" s="6">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6">
         <v>67</v>
       </c>
-      <c r="C16" s="6">
+      <c r="I16" s="6">
+        <v>10</v>
+      </c>
+      <c r="J16" s="10">
         <v>26</v>
       </c>
-      <c r="D16" s="6">
-        <v>20</v>
-      </c>
-      <c r="E16" s="6">
-        <v>68</v>
-      </c>
-      <c r="F16" s="6">
-        <v>2</v>
-      </c>
-      <c r="G16" s="6">
-        <v>62</v>
-      </c>
-      <c r="H16" s="6">
-        <v>12</v>
-      </c>
-      <c r="I16" s="6">
-        <v>20</v>
-      </c>
-      <c r="J16" s="6">
-        <v>95</v>
-      </c>
-      <c r="K16" s="11">
-        <v>63</v>
+      <c r="K16" s="6">
+        <v>38</v>
       </c>
       <c r="L16" s="6">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="M16" s="6">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="N16" s="6">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O16" s="6">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="P16" s="6">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="Q16" s="6">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="R16" s="6">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="S16" s="6">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="T16" s="6">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="U16" s="6">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C17" s="6">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D17" s="6">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="E17" s="6">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="F17" s="6">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6">
+        <v>62</v>
+      </c>
+      <c r="H17" s="6">
+        <v>12</v>
+      </c>
+      <c r="I17" s="6">
+        <v>20</v>
+      </c>
+      <c r="J17" s="6">
+        <v>95</v>
+      </c>
+      <c r="K17" s="10">
+        <v>63</v>
+      </c>
+      <c r="L17" s="6">
+        <v>94</v>
+      </c>
+      <c r="M17" s="6">
+        <v>39</v>
+      </c>
+      <c r="N17" s="6">
+        <v>63</v>
+      </c>
+      <c r="O17" s="6">
+        <v>8</v>
+      </c>
+      <c r="P17" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>91</v>
+      </c>
+      <c r="R17" s="6">
         <v>66</v>
       </c>
-      <c r="G17" s="6">
-        <v>73</v>
-      </c>
-      <c r="H17" s="6">
-        <v>99</v>
-      </c>
-      <c r="I17" s="6">
-        <v>26</v>
-      </c>
-      <c r="J17" s="6">
-        <v>97</v>
-      </c>
-      <c r="K17" s="6">
-        <v>17</v>
-      </c>
-      <c r="L17" s="11">
-        <v>78</v>
-      </c>
-      <c r="M17" s="6">
-        <v>78</v>
-      </c>
-      <c r="N17" s="6">
-        <v>96</v>
-      </c>
-      <c r="O17" s="6">
-        <v>83</v>
-      </c>
-      <c r="P17" s="6">
-        <v>14</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>88</v>
-      </c>
-      <c r="R17" s="6">
-        <v>34</v>
-      </c>
       <c r="S17" s="6">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="T17" s="6">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="U17" s="6">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C18" s="6">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D18" s="6">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E18" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F18" s="6">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G18" s="6">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="H18" s="6">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="I18" s="6">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J18" s="6">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="K18" s="6">
-        <v>45</v>
-      </c>
-      <c r="L18" s="6">
-        <v>35</v>
-      </c>
-      <c r="M18" s="11">
+        <v>17</v>
+      </c>
+      <c r="L18" s="10">
+        <v>78</v>
+      </c>
+      <c r="M18" s="6">
+        <v>78</v>
+      </c>
+      <c r="N18" s="6">
+        <v>96</v>
+      </c>
+      <c r="O18" s="6">
+        <v>83</v>
+      </c>
+      <c r="P18" s="6">
         <v>14</v>
       </c>
-      <c r="N18" s="6">
-        <v>0</v>
-      </c>
-      <c r="O18" s="6">
-        <v>61</v>
-      </c>
-      <c r="P18" s="6">
-        <v>33</v>
-      </c>
       <c r="Q18" s="6">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="R18" s="6">
         <v>34</v>
       </c>
       <c r="S18" s="6">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="T18" s="6">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="U18" s="6">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="C19" s="6">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D19" s="6">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E19" s="6">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F19" s="6">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="G19" s="6">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="H19" s="6">
+        <v>76</v>
+      </c>
+      <c r="I19" s="6">
+        <v>44</v>
+      </c>
+      <c r="J19" s="6">
+        <v>20</v>
+      </c>
+      <c r="K19" s="6">
+        <v>45</v>
+      </c>
+      <c r="L19" s="6">
+        <v>35</v>
+      </c>
+      <c r="M19" s="10">
+        <v>14</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0</v>
+      </c>
+      <c r="O19" s="6">
+        <v>61</v>
+      </c>
+      <c r="P19" s="6">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>97</v>
+      </c>
+      <c r="R19" s="6">
+        <v>34</v>
+      </c>
+      <c r="S19" s="6">
         <v>31</v>
       </c>
-      <c r="I19" s="6">
-        <v>67</v>
-      </c>
-      <c r="J19" s="6">
-        <v>15</v>
-      </c>
-      <c r="K19" s="6">
-        <v>94</v>
-      </c>
-      <c r="L19" s="6">
-        <v>3</v>
-      </c>
-      <c r="M19" s="6">
-        <v>80</v>
-      </c>
-      <c r="N19" s="6">
-        <v>4</v>
-      </c>
-      <c r="O19" s="6">
-        <v>62</v>
-      </c>
-      <c r="P19" s="6">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>14</v>
-      </c>
-      <c r="R19" s="6">
-        <v>9</v>
-      </c>
-      <c r="S19" s="6">
-        <v>53</v>
-      </c>
       <c r="T19" s="6">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="U19" s="6">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" s="6">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C20" s="6">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D20" s="6">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F20" s="6">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="G20" s="6">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="H20" s="6">
         <v>31</v>
       </c>
       <c r="I20" s="6">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="J20" s="6">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="K20" s="6">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="L20" s="6">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="M20" s="6">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="N20" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O20" s="6">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="P20" s="6">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="Q20" s="6">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="R20" s="6">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="S20" s="6">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="T20" s="6">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="U20" s="6">
-        <v>57</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D21" s="6">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6">
+        <v>42</v>
+      </c>
+      <c r="F21" s="6">
+        <v>96</v>
+      </c>
+      <c r="G21" s="6">
+        <v>35</v>
+      </c>
+      <c r="H21" s="6">
+        <v>31</v>
+      </c>
+      <c r="I21" s="6">
+        <v>47</v>
+      </c>
+      <c r="J21" s="6">
+        <v>55</v>
+      </c>
+      <c r="K21" s="6">
+        <v>58</v>
+      </c>
+      <c r="L21" s="6">
+        <v>88</v>
+      </c>
+      <c r="M21" s="6">
+        <v>24</v>
+      </c>
+      <c r="N21" s="6">
         <v>0</v>
       </c>
-      <c r="E21" s="6">
-        <v>48</v>
-      </c>
-      <c r="F21" s="6">
-        <v>35</v>
-      </c>
-      <c r="G21" s="6">
-        <v>71</v>
-      </c>
-      <c r="H21" s="6">
-        <v>89</v>
-      </c>
-      <c r="I21" s="6">
-        <v>7</v>
-      </c>
-      <c r="J21" s="6">
-        <v>5</v>
-      </c>
-      <c r="K21" s="6">
-        <v>44</v>
-      </c>
-      <c r="L21" s="6">
-        <v>44</v>
-      </c>
-      <c r="M21" s="6">
-        <v>37</v>
-      </c>
-      <c r="N21" s="6">
-        <v>44</v>
-      </c>
       <c r="O21" s="6">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="P21" s="6">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="Q21" s="6">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="R21" s="6">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="S21" s="6">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="T21" s="6">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="U21" s="6">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" s="6">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="C22" s="6">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D22" s="6">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E22" s="6">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F22" s="6">
+        <v>35</v>
+      </c>
+      <c r="G22" s="6">
+        <v>71</v>
+      </c>
+      <c r="H22" s="6">
+        <v>89</v>
+      </c>
+      <c r="I22" s="6">
+        <v>7</v>
+      </c>
+      <c r="J22" s="6">
         <v>5</v>
       </c>
-      <c r="G22" s="6">
-        <v>94</v>
-      </c>
-      <c r="H22" s="6">
-        <v>47</v>
-      </c>
-      <c r="I22" s="6">
-        <v>69</v>
-      </c>
-      <c r="J22" s="6">
-        <v>28</v>
-      </c>
       <c r="K22" s="6">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="L22" s="6">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="M22" s="6">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="N22" s="6">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="O22" s="6">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="P22" s="6">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>58</v>
+      </c>
+      <c r="R22" s="6">
+        <v>51</v>
+      </c>
+      <c r="S22" s="6">
+        <v>54</v>
+      </c>
+      <c r="T22" s="6">
         <v>17</v>
       </c>
-      <c r="Q22" s="6">
-        <v>77</v>
-      </c>
-      <c r="R22" s="6">
-        <v>4</v>
-      </c>
-      <c r="S22" s="6">
-        <v>89</v>
-      </c>
-      <c r="T22" s="6">
-        <v>55</v>
-      </c>
       <c r="U22" s="6">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6">
+        <v>80</v>
+      </c>
+      <c r="D23" s="6">
+        <v>81</v>
+      </c>
+      <c r="E23" s="6">
+        <v>68</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="6">
+        <v>94</v>
+      </c>
+      <c r="H23" s="6">
+        <v>47</v>
+      </c>
+      <c r="I23" s="6">
+        <v>69</v>
+      </c>
+      <c r="J23" s="6">
+        <v>28</v>
+      </c>
+      <c r="K23" s="6">
+        <v>73</v>
+      </c>
+      <c r="L23" s="6">
+        <v>92</v>
+      </c>
+      <c r="M23" s="6">
+        <v>13</v>
+      </c>
+      <c r="N23" s="6">
+        <v>86</v>
+      </c>
+      <c r="O23" s="6">
+        <v>52</v>
+      </c>
+      <c r="P23" s="6">
+        <v>17</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>77</v>
+      </c>
+      <c r="R23" s="6">
         <v>4</v>
       </c>
-      <c r="C23" s="6">
-        <v>52</v>
-      </c>
-      <c r="D23" s="6">
-        <v>8</v>
-      </c>
-      <c r="E23" s="6">
-        <v>83</v>
-      </c>
-      <c r="F23" s="6">
-        <v>97</v>
-      </c>
-      <c r="G23" s="6">
-        <v>35</v>
-      </c>
-      <c r="H23" s="6">
-        <v>99</v>
-      </c>
-      <c r="I23" s="6">
-        <v>16</v>
-      </c>
-      <c r="J23" s="6">
-        <v>7</v>
-      </c>
-      <c r="K23" s="6">
-        <v>97</v>
-      </c>
-      <c r="L23" s="6">
-        <v>57</v>
-      </c>
-      <c r="M23" s="6">
-        <v>32</v>
-      </c>
-      <c r="N23" s="6">
-        <v>16</v>
-      </c>
-      <c r="O23" s="6">
-        <v>26</v>
-      </c>
-      <c r="P23" s="6">
-        <v>26</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>79</v>
-      </c>
-      <c r="R23" s="6">
-        <v>33</v>
-      </c>
       <c r="S23" s="6">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="T23" s="6">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="U23" s="6">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B24" s="6">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C24" s="6">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D24" s="6">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E24" s="6">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F24" s="6">
+        <v>97</v>
+      </c>
+      <c r="G24" s="6">
+        <v>35</v>
+      </c>
+      <c r="H24" s="6">
+        <v>99</v>
+      </c>
+      <c r="I24" s="6">
+        <v>16</v>
+      </c>
+      <c r="J24" s="6">
+        <v>7</v>
+      </c>
+      <c r="K24" s="6">
+        <v>97</v>
+      </c>
+      <c r="L24" s="6">
         <v>57</v>
       </c>
-      <c r="G24" s="6">
-        <v>62</v>
-      </c>
-      <c r="H24" s="6">
-        <v>20</v>
-      </c>
-      <c r="I24" s="6">
-        <v>72</v>
-      </c>
-      <c r="J24" s="6">
-        <v>3</v>
-      </c>
-      <c r="K24" s="6">
-        <v>46</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="M24" s="6">
+        <v>32</v>
+      </c>
+      <c r="N24" s="6">
+        <v>16</v>
+      </c>
+      <c r="O24" s="6">
+        <v>26</v>
+      </c>
+      <c r="P24" s="6">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>79</v>
+      </c>
+      <c r="R24" s="6">
         <v>33</v>
       </c>
-      <c r="M24" s="6">
-        <v>67</v>
-      </c>
-      <c r="N24" s="6">
-        <v>46</v>
-      </c>
-      <c r="O24" s="6">
-        <v>55</v>
-      </c>
-      <c r="P24" s="6">
-        <v>12</v>
-      </c>
-      <c r="Q24" s="6">
-        <v>32</v>
-      </c>
-      <c r="R24" s="6">
-        <v>63</v>
-      </c>
       <c r="S24" s="6">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="T24" s="6">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="U24" s="6">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C25" s="6">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="E25" s="6">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="F25" s="6">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G25" s="6">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="H25" s="6">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="I25" s="6">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="J25" s="6">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="K25" s="6">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="L25" s="6">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="M25" s="6">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="N25" s="6">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="O25" s="6">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="P25" s="6">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="Q25" s="6">
         <v>32</v>
       </c>
       <c r="R25" s="6">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="S25" s="6">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="T25" s="6">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="U25" s="6">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C26" s="6">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D26" s="6">
+        <v>16</v>
+      </c>
+      <c r="E26" s="6">
+        <v>73</v>
+      </c>
+      <c r="F26" s="6">
+        <v>38</v>
+      </c>
+      <c r="G26" s="6">
+        <v>25</v>
+      </c>
+      <c r="H26" s="6">
+        <v>39</v>
+      </c>
+      <c r="I26" s="6">
+        <v>11</v>
+      </c>
+      <c r="J26" s="6">
+        <v>24</v>
+      </c>
+      <c r="K26" s="6">
+        <v>94</v>
+      </c>
+      <c r="L26" s="6">
+        <v>72</v>
+      </c>
+      <c r="M26" s="6">
+        <v>18</v>
+      </c>
+      <c r="N26" s="6">
+        <v>8</v>
+      </c>
+      <c r="O26" s="6">
+        <v>46</v>
+      </c>
+      <c r="P26" s="6">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>32</v>
+      </c>
+      <c r="R26" s="6">
+        <v>40</v>
+      </c>
+      <c r="S26" s="6">
+        <v>62</v>
+      </c>
+      <c r="T26" s="6">
+        <v>76</v>
+      </c>
+      <c r="U26" s="6">
         <v>36</v>
-      </c>
-      <c r="E26" s="6">
-        <v>41</v>
-      </c>
-      <c r="F26" s="6">
-        <v>72</v>
-      </c>
-      <c r="G26" s="6">
-        <v>30</v>
-      </c>
-      <c r="H26" s="6">
-        <v>23</v>
-      </c>
-      <c r="I26" s="6">
-        <v>88</v>
-      </c>
-      <c r="J26" s="6">
-        <v>34</v>
-      </c>
-      <c r="K26" s="6">
-        <v>62</v>
-      </c>
-      <c r="L26" s="6">
-        <v>99</v>
-      </c>
-      <c r="M26" s="6">
-        <v>69</v>
-      </c>
-      <c r="N26" s="6">
-        <v>82</v>
-      </c>
-      <c r="O26" s="6">
-        <v>67</v>
-      </c>
-      <c r="P26" s="6">
-        <v>59</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>85</v>
-      </c>
-      <c r="R26" s="6">
-        <v>74</v>
-      </c>
-      <c r="S26" s="6">
-        <v>4</v>
-      </c>
-      <c r="T26" s="6">
-        <v>36</v>
-      </c>
-      <c r="U26" s="6">
-        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.35">
@@ -2140,126 +2105,191 @@
         <v>20</v>
       </c>
       <c r="C27" s="6">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D27" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E27" s="6">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F27" s="6">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G27" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" s="6">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="I27" s="6">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="J27" s="6">
+        <v>34</v>
+      </c>
+      <c r="K27" s="6">
+        <v>62</v>
+      </c>
+      <c r="L27" s="6">
+        <v>99</v>
+      </c>
+      <c r="M27" s="6">
+        <v>69</v>
+      </c>
+      <c r="N27" s="6">
+        <v>82</v>
+      </c>
+      <c r="O27" s="6">
+        <v>67</v>
+      </c>
+      <c r="P27" s="6">
+        <v>59</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>85</v>
+      </c>
+      <c r="R27" s="6">
         <v>74</v>
       </c>
-      <c r="K27" s="6">
-        <v>31</v>
-      </c>
-      <c r="L27" s="6">
-        <v>49</v>
-      </c>
-      <c r="M27" s="6">
-        <v>71</v>
-      </c>
-      <c r="N27" s="6">
-        <v>48</v>
-      </c>
-      <c r="O27" s="6">
-        <v>86</v>
-      </c>
-      <c r="P27" s="6">
-        <v>81</v>
-      </c>
-      <c r="Q27" s="6">
+      <c r="S27" s="6">
+        <v>4</v>
+      </c>
+      <c r="T27" s="6">
+        <v>36</v>
+      </c>
+      <c r="U27" s="6">
         <v>16</v>
-      </c>
-      <c r="R27" s="6">
-        <v>23</v>
-      </c>
-      <c r="S27" s="6">
-        <v>57</v>
-      </c>
-      <c r="T27" s="6">
-        <v>5</v>
-      </c>
-      <c r="U27" s="6">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
+        <v>20</v>
+      </c>
+      <c r="C28" s="6">
+        <v>73</v>
+      </c>
+      <c r="D28" s="6">
+        <v>35</v>
+      </c>
+      <c r="E28" s="6">
+        <v>29</v>
+      </c>
+      <c r="F28" s="6">
+        <v>78</v>
+      </c>
+      <c r="G28" s="6">
+        <v>31</v>
+      </c>
+      <c r="H28" s="6">
+        <v>90</v>
+      </c>
+      <c r="I28" s="6">
         <v>1</v>
       </c>
-      <c r="C28" s="6">
+      <c r="J28" s="6">
+        <v>74</v>
+      </c>
+      <c r="K28" s="6">
+        <v>31</v>
+      </c>
+      <c r="L28" s="6">
+        <v>49</v>
+      </c>
+      <c r="M28" s="6">
+        <v>71</v>
+      </c>
+      <c r="N28" s="6">
+        <v>48</v>
+      </c>
+      <c r="O28" s="6">
+        <v>86</v>
+      </c>
+      <c r="P28" s="6">
+        <v>81</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>16</v>
+      </c>
+      <c r="R28" s="6">
+        <v>23</v>
+      </c>
+      <c r="S28" s="6">
+        <v>57</v>
+      </c>
+      <c r="T28" s="6">
+        <v>5</v>
+      </c>
+      <c r="U28" s="6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6">
         <v>70</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>54</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>71</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F29" s="6">
         <v>83</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G29" s="6">
         <v>51</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H29" s="6">
         <v>54</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I29" s="6">
         <v>69</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J29" s="6">
         <v>16</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K29" s="6">
         <v>92</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L29" s="6">
         <v>33</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M29" s="6">
         <v>48</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N29" s="6">
         <v>61</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O29" s="6">
         <v>43</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P29" s="6">
         <v>52</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q29" s="6">
         <v>1</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R29" s="6">
         <v>89</v>
       </c>
-      <c r="S28" s="6">
+      <c r="S29" s="6">
         <v>19</v>
       </c>
-      <c r="T28" s="6">
+      <c r="T29" s="6">
         <v>67</v>
       </c>
-      <c r="U28" s="6">
+      <c r="U29" s="6">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{A776FA43-552E-4EBD-A1DF-28FC3A0E926C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2269,10 +2299,10 @@
   <dimension ref="B5:AQ64"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -8649,13 +8679,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D608A6F-8481-498F-959A-C5D3AB51DD5E}">
-  <dimension ref="B2:W30"/>
+  <dimension ref="B2:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="23" width="3.90625" customWidth="1"/>
@@ -8666,1283 +8696,1260 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B4" s="5">
         <f ca="1">_xlfn.LET(
-_xlpm.MAX_HORIZONTAL, MAX(_xlfn.MAP(D11:T30,_xlfn.LAMBDA(_xlpm.CELL, PRODUCT(OFFSET(_xlpm.CELL,0,0,1,4))))),
-_xlpm.MAX_VERTICAL, MAX(_xlfn.MAP(D11:W27,_xlfn.LAMBDA(_xlpm.CELL, PRODUCT(OFFSET(_xlpm.CELL,0,0,4,1))))),
-_xlpm.MAX_DIAGONAL_1, MAX(_xlfn.MAP(D11:T27,_xlfn.LAMBDA(_xlpm.CELL,PRODUCT(_xlpm.CELL,OFFSET(_xlpm.CELL,1,1),OFFSET(_xlpm.CELL,2,2),OFFSET(_xlpm.CELL,3,3))))),
-_xlpm.MAX_DIAGONAL_2, MAX(_xlfn.MAP(D14:T30,_xlfn.LAMBDA(_xlpm.CELL,PRODUCT(_xlpm.CELL,OFFSET(_xlpm.CELL,-1,1),OFFSET(_xlpm.CELL,-2,2),OFFSET(_xlpm.CELL,-3,3))))),
+_xlpm.MAX_HORIZONTAL, MAX(_xlfn.MAP(D6:T25,_xlfn.LAMBDA(_xlpm.CELL, PRODUCT(OFFSET(_xlpm.CELL,0,0,1,4))))),
+_xlpm.MAX_VERTICAL, MAX(_xlfn.MAP(D6:W22,_xlfn.LAMBDA(_xlpm.CELL, PRODUCT(OFFSET(_xlpm.CELL,0,0,4,1))))),
+_xlpm.MAX_DIAGONAL_1, MAX(_xlfn.MAP(D6:T22,_xlfn.LAMBDA(_xlpm.CELL,PRODUCT(_xlpm.CELL,OFFSET(_xlpm.CELL,1,1),OFFSET(_xlpm.CELL,2,2),OFFSET(_xlpm.CELL,3,3))))),
+_xlpm.MAX_DIAGONAL_2, MAX(_xlfn.MAP(D9:T25,_xlfn.LAMBDA(_xlpm.CELL,PRODUCT(_xlpm.CELL,OFFSET(_xlpm.CELL,-1,1),OFFSET(_xlpm.CELL,-2,2),OFFSET(_xlpm.CELL,-3,3))))),
 MAX(_xlpm.MAX_HORIZONTAL, _xlpm.MAX_VERTICAL,_xlpm.MAX_DIAGONAL_1,_xlpm.MAX_DIAGONAL_2))</f>
         <v>70600674</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="D6" s="6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6">
+        <v>97</v>
+      </c>
+      <c r="H6" s="6">
+        <v>38</v>
+      </c>
+      <c r="I6" s="6">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>40</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>75</v>
+      </c>
+      <c r="N6" s="6">
+        <v>4</v>
+      </c>
+      <c r="O6" s="6">
+        <v>5</v>
+      </c>
+      <c r="P6" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>78</v>
+      </c>
+      <c r="R6" s="6">
+        <v>52</v>
+      </c>
+      <c r="S6" s="6">
+        <v>12</v>
+      </c>
+      <c r="T6" s="6">
+        <v>50</v>
+      </c>
+      <c r="U6" s="6">
+        <v>77</v>
+      </c>
+      <c r="V6" s="6">
+        <v>91</v>
+      </c>
+      <c r="W6" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="D7" s="6">
+        <v>49</v>
+      </c>
+      <c r="E7" s="6">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6">
+        <v>99</v>
+      </c>
+      <c r="G7" s="6">
+        <v>40</v>
+      </c>
+      <c r="H7" s="6">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6">
+        <v>81</v>
+      </c>
+      <c r="J7" s="6">
+        <v>18</v>
+      </c>
+      <c r="K7" s="6">
+        <v>57</v>
+      </c>
+      <c r="L7" s="6">
+        <v>60</v>
+      </c>
+      <c r="M7" s="6">
+        <v>87</v>
+      </c>
+      <c r="N7" s="6">
+        <v>17</v>
+      </c>
+      <c r="O7" s="6">
+        <v>40</v>
+      </c>
+      <c r="P7" s="6">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>43</v>
+      </c>
+      <c r="R7" s="6">
+        <v>69</v>
+      </c>
+      <c r="S7" s="6">
+        <v>48</v>
+      </c>
+      <c r="T7" s="6">
+        <v>4</v>
+      </c>
+      <c r="U7" s="6">
+        <v>56</v>
+      </c>
+      <c r="V7" s="6">
+        <v>62</v>
+      </c>
+      <c r="W7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="D8" s="6">
+        <v>81</v>
+      </c>
+      <c r="E8" s="6">
+        <v>49</v>
+      </c>
+      <c r="F8" s="6">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6">
+        <v>73</v>
+      </c>
+      <c r="H8" s="6">
+        <v>55</v>
+      </c>
+      <c r="I8" s="6">
+        <v>79</v>
+      </c>
+      <c r="J8" s="6">
+        <v>14</v>
+      </c>
+      <c r="K8" s="6">
+        <v>29</v>
+      </c>
+      <c r="L8" s="6">
+        <v>93</v>
+      </c>
+      <c r="M8" s="6">
+        <v>71</v>
+      </c>
+      <c r="N8" s="6">
+        <v>40</v>
+      </c>
+      <c r="O8" s="6">
+        <v>67</v>
+      </c>
+      <c r="P8" s="6">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>88</v>
+      </c>
+      <c r="R8" s="6">
+        <v>30</v>
+      </c>
+      <c r="S8" s="6">
+        <v>3</v>
+      </c>
+      <c r="T8" s="6">
+        <v>49</v>
+      </c>
+      <c r="U8" s="6">
+        <v>13</v>
+      </c>
+      <c r="V8" s="6">
+        <v>36</v>
+      </c>
+      <c r="W8" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="D9" s="6">
+        <v>52</v>
+      </c>
+      <c r="E9" s="6">
+        <v>70</v>
+      </c>
+      <c r="F9" s="6">
+        <v>95</v>
+      </c>
+      <c r="G9" s="6">
+        <v>23</v>
+      </c>
+      <c r="H9" s="6">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6">
+        <v>60</v>
+      </c>
+      <c r="J9" s="6">
+        <v>11</v>
+      </c>
+      <c r="K9" s="6">
+        <v>42</v>
+      </c>
+      <c r="L9" s="6">
+        <v>69</v>
+      </c>
+      <c r="M9" s="6">
+        <v>24</v>
+      </c>
+      <c r="N9" s="6">
+        <v>68</v>
+      </c>
+      <c r="O9" s="6">
+        <v>56</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>32</v>
+      </c>
+      <c r="R9" s="6">
+        <v>56</v>
+      </c>
+      <c r="S9" s="6">
+        <v>71</v>
+      </c>
+      <c r="T9" s="6">
+        <v>37</v>
+      </c>
+      <c r="U9" s="6">
+        <v>2</v>
+      </c>
+      <c r="V9" s="6">
+        <v>36</v>
+      </c>
+      <c r="W9" s="6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="D10" s="6">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6">
+        <v>71</v>
+      </c>
+      <c r="H10" s="6">
+        <v>51</v>
+      </c>
+      <c r="I10" s="6">
+        <v>67</v>
+      </c>
+      <c r="J10" s="6">
+        <v>63</v>
+      </c>
+      <c r="K10" s="6">
+        <v>89</v>
+      </c>
+      <c r="L10" s="6">
+        <v>41</v>
+      </c>
+      <c r="M10" s="6">
+        <v>92</v>
+      </c>
+      <c r="N10" s="6">
+        <v>36</v>
+      </c>
+      <c r="O10" s="6">
+        <v>54</v>
+      </c>
+      <c r="P10" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>40</v>
+      </c>
+      <c r="R10" s="6">
+        <v>40</v>
+      </c>
+      <c r="S10" s="6">
+        <v>28</v>
+      </c>
+      <c r="T10" s="6">
+        <v>66</v>
+      </c>
+      <c r="U10" s="6">
+        <v>33</v>
+      </c>
+      <c r="V10" s="6">
+        <v>13</v>
+      </c>
+      <c r="W10" s="6">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D11" s="6">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6">
+        <v>32</v>
+      </c>
+      <c r="G11" s="6">
+        <v>60</v>
+      </c>
+      <c r="H11" s="6">
+        <v>99</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>45</v>
+      </c>
+      <c r="K11" s="11">
         <v>2</v>
       </c>
-      <c r="F11" s="6">
-        <v>22</v>
-      </c>
-      <c r="G11" s="6">
-        <v>97</v>
-      </c>
-      <c r="H11" s="6">
-        <v>38</v>
-      </c>
-      <c r="I11" s="6">
-        <v>15</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>40</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
+      <c r="L11" s="11">
+        <v>44</v>
+      </c>
+      <c r="M11" s="11">
         <v>75</v>
       </c>
-      <c r="N11" s="6">
-        <v>4</v>
-      </c>
-      <c r="O11" s="6">
-        <v>5</v>
-      </c>
-      <c r="P11" s="6">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="6">
+      <c r="N11" s="11">
+        <v>33</v>
+      </c>
+      <c r="O11" s="11">
+        <v>53</v>
+      </c>
+      <c r="P11" s="11">
         <v>78</v>
       </c>
-      <c r="R11" s="6">
-        <v>52</v>
+      <c r="Q11" s="11">
+        <v>36</v>
+      </c>
+      <c r="R11" s="11">
+        <v>84</v>
       </c>
       <c r="S11" s="6">
+        <v>20</v>
+      </c>
+      <c r="T11" s="6">
+        <v>35</v>
+      </c>
+      <c r="U11" s="6">
+        <v>17</v>
+      </c>
+      <c r="V11" s="6">
         <v>12</v>
       </c>
-      <c r="T11" s="6">
+      <c r="W11" s="6">
         <v>50</v>
-      </c>
-      <c r="U11" s="6">
-        <v>77</v>
-      </c>
-      <c r="V11" s="6">
-        <v>91</v>
-      </c>
-      <c r="W11" s="6">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D12" s="6">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="F12" s="6">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G12" s="6">
+        <v>28</v>
+      </c>
+      <c r="H12" s="6">
+        <v>64</v>
+      </c>
+      <c r="I12" s="6">
+        <v>23</v>
+      </c>
+      <c r="J12" s="6">
+        <v>67</v>
+      </c>
+      <c r="K12" s="11">
+        <v>10</v>
+      </c>
+      <c r="L12" s="11">
+        <v>26</v>
+      </c>
+      <c r="M12" s="11">
+        <v>38</v>
+      </c>
+      <c r="N12" s="11">
         <v>40</v>
       </c>
-      <c r="H12" s="6">
-        <v>17</v>
-      </c>
-      <c r="I12" s="6">
-        <v>81</v>
-      </c>
-      <c r="J12" s="6">
+      <c r="O12" s="11">
+        <v>67</v>
+      </c>
+      <c r="P12" s="11">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>54</v>
+      </c>
+      <c r="R12" s="11">
+        <v>70</v>
+      </c>
+      <c r="S12" s="6">
+        <v>66</v>
+      </c>
+      <c r="T12" s="6">
         <v>18</v>
       </c>
-      <c r="K12" s="6">
-        <v>57</v>
-      </c>
-      <c r="L12" s="6">
-        <v>60</v>
-      </c>
-      <c r="M12" s="6">
-        <v>87</v>
-      </c>
-      <c r="N12" s="6">
-        <v>17</v>
-      </c>
-      <c r="O12" s="6">
-        <v>40</v>
-      </c>
-      <c r="P12" s="6">
-        <v>98</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>43</v>
-      </c>
-      <c r="R12" s="6">
-        <v>69</v>
-      </c>
-      <c r="S12" s="6">
-        <v>48</v>
-      </c>
-      <c r="T12" s="6">
-        <v>4</v>
-      </c>
       <c r="U12" s="6">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="V12" s="6">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="W12" s="6">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D13" s="6">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E13" s="6">
+        <v>26</v>
+      </c>
+      <c r="F13" s="6">
+        <v>20</v>
+      </c>
+      <c r="G13" s="6">
+        <v>68</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>62</v>
+      </c>
+      <c r="J13" s="6">
+        <v>12</v>
+      </c>
+      <c r="K13" s="11">
+        <v>20</v>
+      </c>
+      <c r="L13" s="11">
+        <v>95</v>
+      </c>
+      <c r="M13" s="11">
+        <v>63</v>
+      </c>
+      <c r="N13" s="11">
+        <v>94</v>
+      </c>
+      <c r="O13" s="11">
+        <v>39</v>
+      </c>
+      <c r="P13" s="11">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>8</v>
+      </c>
+      <c r="R13" s="11">
+        <v>40</v>
+      </c>
+      <c r="S13" s="6">
+        <v>91</v>
+      </c>
+      <c r="T13" s="6">
+        <v>66</v>
+      </c>
+      <c r="U13" s="6">
         <v>49</v>
       </c>
-      <c r="F13" s="6">
-        <v>31</v>
-      </c>
-      <c r="G13" s="6">
-        <v>73</v>
-      </c>
-      <c r="H13" s="6">
-        <v>55</v>
-      </c>
-      <c r="I13" s="6">
-        <v>79</v>
-      </c>
-      <c r="J13" s="6">
-        <v>14</v>
-      </c>
-      <c r="K13" s="6">
-        <v>29</v>
-      </c>
-      <c r="L13" s="6">
-        <v>93</v>
-      </c>
-      <c r="M13" s="6">
-        <v>71</v>
-      </c>
-      <c r="N13" s="6">
-        <v>40</v>
-      </c>
-      <c r="O13" s="6">
-        <v>67</v>
-      </c>
-      <c r="P13" s="6">
-        <v>53</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>88</v>
-      </c>
-      <c r="R13" s="6">
-        <v>30</v>
-      </c>
-      <c r="S13" s="6">
-        <v>3</v>
-      </c>
-      <c r="T13" s="6">
-        <v>49</v>
-      </c>
-      <c r="U13" s="6">
-        <v>13</v>
-      </c>
       <c r="V13" s="6">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="W13" s="6">
-        <v>65</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D14" s="6">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E14" s="6">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F14" s="6">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="G14" s="6">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H14" s="6">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="I14" s="6">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="J14" s="6">
-        <v>11</v>
-      </c>
-      <c r="K14" s="6">
-        <v>42</v>
-      </c>
-      <c r="L14" s="6">
-        <v>69</v>
-      </c>
-      <c r="M14" s="6">
-        <v>24</v>
-      </c>
-      <c r="N14" s="6">
-        <v>68</v>
-      </c>
-      <c r="O14" s="6">
-        <v>56</v>
-      </c>
-      <c r="P14" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>32</v>
-      </c>
-      <c r="R14" s="6">
-        <v>56</v>
+        <v>99</v>
+      </c>
+      <c r="K14" s="11">
+        <v>26</v>
+      </c>
+      <c r="L14" s="11">
+        <v>97</v>
+      </c>
+      <c r="M14" s="11">
+        <v>17</v>
+      </c>
+      <c r="N14" s="11">
+        <v>78</v>
+      </c>
+      <c r="O14" s="11">
+        <v>78</v>
+      </c>
+      <c r="P14" s="11">
+        <v>96</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>83</v>
+      </c>
+      <c r="R14" s="11">
+        <v>14</v>
       </c>
       <c r="S14" s="6">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="T14" s="6">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U14" s="6">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="V14" s="6">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="W14" s="6">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D15" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6">
+        <v>36</v>
+      </c>
+      <c r="F15" s="6">
+        <v>23</v>
+      </c>
+      <c r="G15" s="6">
+        <v>9</v>
+      </c>
+      <c r="H15" s="6">
+        <v>75</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
+        <v>76</v>
+      </c>
+      <c r="K15" s="11">
+        <v>44</v>
+      </c>
+      <c r="L15" s="11">
+        <v>20</v>
+      </c>
+      <c r="M15" s="11">
+        <v>45</v>
+      </c>
+      <c r="N15" s="11">
+        <v>35</v>
+      </c>
+      <c r="O15" s="11">
+        <v>14</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>61</v>
+      </c>
+      <c r="R15" s="11">
+        <v>33</v>
+      </c>
+      <c r="S15" s="6">
+        <v>97</v>
+      </c>
+      <c r="T15" s="6">
+        <v>34</v>
+      </c>
+      <c r="U15" s="6">
         <v>31</v>
       </c>
-      <c r="F15" s="6">
-        <v>16</v>
-      </c>
-      <c r="G15" s="6">
-        <v>71</v>
-      </c>
-      <c r="H15" s="6">
-        <v>51</v>
-      </c>
-      <c r="I15" s="6">
-        <v>67</v>
-      </c>
-      <c r="J15" s="6">
-        <v>63</v>
-      </c>
-      <c r="K15" s="6">
-        <v>89</v>
-      </c>
-      <c r="L15" s="6">
-        <v>41</v>
-      </c>
-      <c r="M15" s="6">
-        <v>92</v>
-      </c>
-      <c r="N15" s="6">
-        <v>36</v>
-      </c>
-      <c r="O15" s="6">
-        <v>54</v>
-      </c>
-      <c r="P15" s="6">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>40</v>
-      </c>
-      <c r="R15" s="6">
-        <v>40</v>
-      </c>
-      <c r="S15" s="6">
-        <v>28</v>
-      </c>
-      <c r="T15" s="6">
-        <v>66</v>
-      </c>
-      <c r="U15" s="6">
+      <c r="V15" s="6">
         <v>33</v>
       </c>
-      <c r="V15" s="6">
-        <v>13</v>
-      </c>
       <c r="W15" s="6">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D16" s="6">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="E16" s="6">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F16" s="6">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G16" s="6">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="H16" s="6">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="I16" s="6">
+        <v>75</v>
+      </c>
+      <c r="J16" s="6">
+        <v>31</v>
+      </c>
+      <c r="K16" s="11">
+        <v>67</v>
+      </c>
+      <c r="L16" s="11">
+        <v>15</v>
+      </c>
+      <c r="M16" s="11">
+        <v>94</v>
+      </c>
+      <c r="N16" s="11">
         <v>3</v>
       </c>
-      <c r="J16" s="6">
-        <v>45</v>
-      </c>
-      <c r="K16" s="12">
-        <v>2</v>
-      </c>
-      <c r="L16" s="12">
-        <v>44</v>
-      </c>
-      <c r="M16" s="12">
-        <v>75</v>
-      </c>
-      <c r="N16" s="12">
-        <v>33</v>
-      </c>
-      <c r="O16" s="12">
+      <c r="O16" s="11">
+        <v>80</v>
+      </c>
+      <c r="P16" s="11">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>62</v>
+      </c>
+      <c r="R16" s="11">
+        <v>16</v>
+      </c>
+      <c r="S16" s="6">
+        <v>14</v>
+      </c>
+      <c r="T16" s="6">
+        <v>9</v>
+      </c>
+      <c r="U16" s="6">
         <v>53</v>
       </c>
-      <c r="P16" s="12">
-        <v>78</v>
-      </c>
-      <c r="Q16" s="12">
-        <v>36</v>
-      </c>
-      <c r="R16" s="12">
-        <v>84</v>
-      </c>
-      <c r="S16" s="6">
-        <v>20</v>
-      </c>
-      <c r="T16" s="6">
-        <v>35</v>
-      </c>
-      <c r="U16" s="6">
-        <v>17</v>
-      </c>
       <c r="V16" s="6">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="W16" s="6">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D17" s="6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E17" s="6">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="F17" s="6">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="G17" s="6">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H17" s="6">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="I17" s="6">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="J17" s="6">
-        <v>67</v>
-      </c>
-      <c r="K17" s="12">
-        <v>10</v>
-      </c>
-      <c r="L17" s="12">
-        <v>26</v>
-      </c>
-      <c r="M17" s="12">
-        <v>38</v>
-      </c>
-      <c r="N17" s="12">
-        <v>40</v>
-      </c>
-      <c r="O17" s="12">
-        <v>67</v>
-      </c>
-      <c r="P17" s="12">
-        <v>59</v>
-      </c>
-      <c r="Q17" s="12">
+        <v>31</v>
+      </c>
+      <c r="K17" s="6">
+        <v>47</v>
+      </c>
+      <c r="L17" s="6">
+        <v>55</v>
+      </c>
+      <c r="M17" s="6">
+        <v>58</v>
+      </c>
+      <c r="N17" s="6">
+        <v>88</v>
+      </c>
+      <c r="O17" s="6">
+        <v>24</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>17</v>
+      </c>
+      <c r="R17" s="6">
         <v>54</v>
       </c>
-      <c r="R17" s="12">
-        <v>70</v>
-      </c>
       <c r="S17" s="6">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="T17" s="6">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="U17" s="6">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="V17" s="6">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="W17" s="6">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D18" s="6">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="E18" s="6">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F18" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G18" s="6">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="H18" s="6">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="I18" s="6">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="J18" s="6">
-        <v>12</v>
-      </c>
-      <c r="K18" s="12">
-        <v>20</v>
-      </c>
-      <c r="L18" s="12">
-        <v>95</v>
-      </c>
-      <c r="M18" s="12">
-        <v>63</v>
-      </c>
-      <c r="N18" s="12">
-        <v>94</v>
-      </c>
-      <c r="O18" s="12">
-        <v>39</v>
-      </c>
-      <c r="P18" s="12">
-        <v>63</v>
-      </c>
-      <c r="Q18" s="12">
-        <v>8</v>
-      </c>
-      <c r="R18" s="12">
-        <v>40</v>
+        <v>89</v>
+      </c>
+      <c r="K18" s="6">
+        <v>7</v>
+      </c>
+      <c r="L18" s="6">
+        <v>5</v>
+      </c>
+      <c r="M18" s="6">
+        <v>44</v>
+      </c>
+      <c r="N18" s="6">
+        <v>44</v>
+      </c>
+      <c r="O18" s="6">
+        <v>37</v>
+      </c>
+      <c r="P18" s="6">
+        <v>44</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>60</v>
+      </c>
+      <c r="R18" s="6">
+        <v>21</v>
       </c>
       <c r="S18" s="6">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="T18" s="6">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="U18" s="6">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="V18" s="6">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="W18" s="6">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D19" s="6">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E19" s="6">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F19" s="6">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="G19" s="6">
+        <v>68</v>
+      </c>
+      <c r="H19" s="6">
         <v>5</v>
       </c>
-      <c r="H19" s="6">
-        <v>66</v>
-      </c>
       <c r="I19" s="6">
+        <v>94</v>
+      </c>
+      <c r="J19" s="6">
+        <v>47</v>
+      </c>
+      <c r="K19" s="6">
+        <v>69</v>
+      </c>
+      <c r="L19" s="6">
+        <v>28</v>
+      </c>
+      <c r="M19" s="6">
         <v>73</v>
       </c>
-      <c r="J19" s="6">
-        <v>99</v>
-      </c>
-      <c r="K19" s="12">
-        <v>26</v>
-      </c>
-      <c r="L19" s="12">
-        <v>97</v>
-      </c>
-      <c r="M19" s="12">
+      <c r="N19" s="6">
+        <v>92</v>
+      </c>
+      <c r="O19" s="6">
+        <v>13</v>
+      </c>
+      <c r="P19" s="6">
+        <v>86</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>52</v>
+      </c>
+      <c r="R19" s="6">
         <v>17</v>
       </c>
-      <c r="N19" s="12">
-        <v>78</v>
-      </c>
-      <c r="O19" s="12">
-        <v>78</v>
-      </c>
-      <c r="P19" s="12">
-        <v>96</v>
-      </c>
-      <c r="Q19" s="12">
-        <v>83</v>
-      </c>
-      <c r="R19" s="12">
-        <v>14</v>
-      </c>
       <c r="S19" s="6">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="T19" s="6">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="U19" s="6">
         <v>89</v>
       </c>
       <c r="V19" s="6">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="W19" s="6">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D20" s="6">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E20" s="6">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F20" s="6">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G20" s="6">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="H20" s="6">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="I20" s="6">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J20" s="6">
-        <v>76</v>
-      </c>
-      <c r="K20" s="12">
-        <v>44</v>
-      </c>
-      <c r="L20" s="12">
-        <v>20</v>
-      </c>
-      <c r="M20" s="12">
-        <v>45</v>
-      </c>
-      <c r="N20" s="12">
-        <v>35</v>
-      </c>
-      <c r="O20" s="12">
-        <v>14</v>
-      </c>
-      <c r="P20" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="12">
-        <v>61</v>
-      </c>
-      <c r="R20" s="12">
+        <v>99</v>
+      </c>
+      <c r="K20" s="6">
+        <v>16</v>
+      </c>
+      <c r="L20" s="6">
+        <v>7</v>
+      </c>
+      <c r="M20" s="6">
+        <v>97</v>
+      </c>
+      <c r="N20" s="6">
+        <v>57</v>
+      </c>
+      <c r="O20" s="6">
+        <v>32</v>
+      </c>
+      <c r="P20" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>26</v>
+      </c>
+      <c r="R20" s="6">
+        <v>26</v>
+      </c>
+      <c r="S20" s="6">
+        <v>79</v>
+      </c>
+      <c r="T20" s="6">
         <v>33</v>
       </c>
-      <c r="S20" s="6">
-        <v>97</v>
-      </c>
-      <c r="T20" s="6">
-        <v>34</v>
-      </c>
       <c r="U20" s="6">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="V20" s="6">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="W20" s="6">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D21" s="6">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E21" s="6">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F21" s="6">
+        <v>68</v>
+      </c>
+      <c r="G21" s="6">
+        <v>87</v>
+      </c>
+      <c r="H21" s="6">
+        <v>57</v>
+      </c>
+      <c r="I21" s="6">
+        <v>62</v>
+      </c>
+      <c r="J21" s="6">
+        <v>20</v>
+      </c>
+      <c r="K21" s="6">
+        <v>72</v>
+      </c>
+      <c r="L21" s="6">
+        <v>3</v>
+      </c>
+      <c r="M21" s="6">
+        <v>46</v>
+      </c>
+      <c r="N21" s="6">
+        <v>33</v>
+      </c>
+      <c r="O21" s="6">
+        <v>67</v>
+      </c>
+      <c r="P21" s="6">
+        <v>46</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>55</v>
+      </c>
+      <c r="R21" s="6">
+        <v>12</v>
+      </c>
+      <c r="S21" s="6">
+        <v>32</v>
+      </c>
+      <c r="T21" s="6">
+        <v>63</v>
+      </c>
+      <c r="U21" s="6">
+        <v>93</v>
+      </c>
+      <c r="V21" s="6">
         <v>53</v>
       </c>
-      <c r="G21" s="6">
-        <v>28</v>
-      </c>
-      <c r="H21" s="6">
-        <v>22</v>
-      </c>
-      <c r="I21" s="6">
-        <v>75</v>
-      </c>
-      <c r="J21" s="6">
-        <v>31</v>
-      </c>
-      <c r="K21" s="12">
-        <v>67</v>
-      </c>
-      <c r="L21" s="12">
-        <v>15</v>
-      </c>
-      <c r="M21" s="12">
-        <v>94</v>
-      </c>
-      <c r="N21" s="12">
-        <v>3</v>
-      </c>
-      <c r="O21" s="12">
-        <v>80</v>
-      </c>
-      <c r="P21" s="12">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="12">
-        <v>62</v>
-      </c>
-      <c r="R21" s="12">
-        <v>16</v>
-      </c>
-      <c r="S21" s="6">
-        <v>14</v>
-      </c>
-      <c r="T21" s="6">
-        <v>9</v>
-      </c>
-      <c r="U21" s="6">
-        <v>53</v>
-      </c>
-      <c r="V21" s="6">
-        <v>56</v>
-      </c>
       <c r="W21" s="6">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D22" s="6">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6">
+        <v>42</v>
+      </c>
+      <c r="F22" s="6">
         <v>16</v>
       </c>
-      <c r="E22" s="6">
+      <c r="G22" s="6">
+        <v>73</v>
+      </c>
+      <c r="H22" s="6">
+        <v>38</v>
+      </c>
+      <c r="I22" s="6">
+        <v>25</v>
+      </c>
+      <c r="J22" s="6">
         <v>39</v>
       </c>
-      <c r="F22" s="6">
-        <v>5</v>
-      </c>
-      <c r="G22" s="6">
-        <v>42</v>
-      </c>
-      <c r="H22" s="6">
-        <v>96</v>
-      </c>
-      <c r="I22" s="6">
-        <v>35</v>
-      </c>
-      <c r="J22" s="6">
-        <v>31</v>
-      </c>
       <c r="K22" s="6">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="L22" s="6">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="M22" s="6">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="N22" s="6">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="O22" s="6">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="P22" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q22" s="6">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="R22" s="6">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="S22" s="6">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="T22" s="6">
+        <v>40</v>
+      </c>
+      <c r="U22" s="6">
+        <v>62</v>
+      </c>
+      <c r="V22" s="6">
+        <v>76</v>
+      </c>
+      <c r="W22" s="6">
         <v>36</v>
-      </c>
-      <c r="U22" s="6">
-        <v>29</v>
-      </c>
-      <c r="V22" s="6">
-        <v>85</v>
-      </c>
-      <c r="W22" s="6">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D23" s="6">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E23" s="6">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F23" s="6">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G23" s="6">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H23" s="6">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="I23" s="6">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="J23" s="6">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="K23" s="6">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="L23" s="6">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="M23" s="6">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="N23" s="6">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="O23" s="6">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="P23" s="6">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="Q23" s="6">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="R23" s="6">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="S23" s="6">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="T23" s="6">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="U23" s="6">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="V23" s="6">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="W23" s="6">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D24" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24" s="6">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F24" s="6">
+        <v>35</v>
+      </c>
+      <c r="G24" s="6">
+        <v>29</v>
+      </c>
+      <c r="H24" s="6">
+        <v>78</v>
+      </c>
+      <c r="I24" s="6">
+        <v>31</v>
+      </c>
+      <c r="J24" s="6">
+        <v>90</v>
+      </c>
+      <c r="K24" s="6">
+        <v>1</v>
+      </c>
+      <c r="L24" s="6">
+        <v>74</v>
+      </c>
+      <c r="M24" s="6">
+        <v>31</v>
+      </c>
+      <c r="N24" s="6">
+        <v>49</v>
+      </c>
+      <c r="O24" s="6">
+        <v>71</v>
+      </c>
+      <c r="P24" s="6">
+        <v>48</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>86</v>
+      </c>
+      <c r="R24" s="6">
         <v>81</v>
       </c>
-      <c r="G24" s="6">
-        <v>68</v>
-      </c>
-      <c r="H24" s="6">
+      <c r="S24" s="6">
+        <v>16</v>
+      </c>
+      <c r="T24" s="6">
+        <v>23</v>
+      </c>
+      <c r="U24" s="6">
+        <v>57</v>
+      </c>
+      <c r="V24" s="6">
         <v>5</v>
       </c>
-      <c r="I24" s="6">
-        <v>94</v>
-      </c>
-      <c r="J24" s="6">
-        <v>47</v>
-      </c>
-      <c r="K24" s="6">
-        <v>69</v>
-      </c>
-      <c r="L24" s="6">
-        <v>28</v>
-      </c>
-      <c r="M24" s="6">
-        <v>73</v>
-      </c>
-      <c r="N24" s="6">
-        <v>92</v>
-      </c>
-      <c r="O24" s="6">
-        <v>13</v>
-      </c>
-      <c r="P24" s="6">
-        <v>86</v>
-      </c>
-      <c r="Q24" s="6">
-        <v>52</v>
-      </c>
-      <c r="R24" s="6">
-        <v>17</v>
-      </c>
-      <c r="S24" s="6">
-        <v>77</v>
-      </c>
-      <c r="T24" s="6">
-        <v>4</v>
-      </c>
-      <c r="U24" s="6">
-        <v>89</v>
-      </c>
-      <c r="V24" s="6">
-        <v>55</v>
-      </c>
       <c r="W24" s="6">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D25" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" s="6">
+        <v>70</v>
+      </c>
+      <c r="F25" s="6">
+        <v>54</v>
+      </c>
+      <c r="G25" s="6">
+        <v>71</v>
+      </c>
+      <c r="H25" s="6">
+        <v>83</v>
+      </c>
+      <c r="I25" s="6">
+        <v>51</v>
+      </c>
+      <c r="J25" s="6">
+        <v>54</v>
+      </c>
+      <c r="K25" s="6">
+        <v>69</v>
+      </c>
+      <c r="L25" s="6">
+        <v>16</v>
+      </c>
+      <c r="M25" s="6">
+        <v>92</v>
+      </c>
+      <c r="N25" s="6">
+        <v>33</v>
+      </c>
+      <c r="O25" s="6">
+        <v>48</v>
+      </c>
+      <c r="P25" s="6">
+        <v>61</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>43</v>
+      </c>
+      <c r="R25" s="6">
         <v>52</v>
       </c>
-      <c r="F25" s="6">
-        <v>8</v>
-      </c>
-      <c r="G25" s="6">
-        <v>83</v>
-      </c>
-      <c r="H25" s="6">
-        <v>97</v>
-      </c>
-      <c r="I25" s="6">
-        <v>35</v>
-      </c>
-      <c r="J25" s="6">
-        <v>99</v>
-      </c>
-      <c r="K25" s="6">
-        <v>16</v>
-      </c>
-      <c r="L25" s="6">
-        <v>7</v>
-      </c>
-      <c r="M25" s="6">
-        <v>97</v>
-      </c>
-      <c r="N25" s="6">
-        <v>57</v>
-      </c>
-      <c r="O25" s="6">
-        <v>32</v>
-      </c>
-      <c r="P25" s="6">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>26</v>
-      </c>
-      <c r="R25" s="6">
-        <v>26</v>
-      </c>
       <c r="S25" s="6">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="T25" s="6">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="U25" s="6">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="V25" s="6">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="W25" s="6">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D26" s="6">
-        <v>88</v>
-      </c>
-      <c r="E26" s="6">
-        <v>36</v>
-      </c>
-      <c r="F26" s="6">
-        <v>68</v>
-      </c>
-      <c r="G26" s="6">
-        <v>87</v>
-      </c>
-      <c r="H26" s="6">
-        <v>57</v>
-      </c>
-      <c r="I26" s="6">
-        <v>62</v>
-      </c>
-      <c r="J26" s="6">
-        <v>20</v>
-      </c>
-      <c r="K26" s="6">
-        <v>72</v>
-      </c>
-      <c r="L26" s="6">
-        <v>3</v>
-      </c>
-      <c r="M26" s="6">
-        <v>46</v>
-      </c>
-      <c r="N26" s="6">
-        <v>33</v>
-      </c>
-      <c r="O26" s="6">
-        <v>67</v>
-      </c>
-      <c r="P26" s="6">
-        <v>46</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>55</v>
-      </c>
-      <c r="R26" s="6">
-        <v>12</v>
-      </c>
-      <c r="S26" s="6">
-        <v>32</v>
-      </c>
-      <c r="T26" s="6">
-        <v>63</v>
-      </c>
-      <c r="U26" s="6">
-        <v>93</v>
-      </c>
-      <c r="V26" s="6">
-        <v>53</v>
-      </c>
-      <c r="W26" s="6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D27" s="6">
-        <v>4</v>
-      </c>
-      <c r="E27" s="6">
-        <v>42</v>
-      </c>
-      <c r="F27" s="6">
-        <v>16</v>
-      </c>
-      <c r="G27" s="6">
-        <v>73</v>
-      </c>
-      <c r="H27" s="6">
-        <v>38</v>
-      </c>
-      <c r="I27" s="6">
-        <v>25</v>
-      </c>
-      <c r="J27" s="6">
-        <v>39</v>
-      </c>
-      <c r="K27" s="6">
-        <v>11</v>
-      </c>
-      <c r="L27" s="6">
-        <v>24</v>
-      </c>
-      <c r="M27" s="6">
-        <v>94</v>
-      </c>
-      <c r="N27" s="6">
-        <v>72</v>
-      </c>
-      <c r="O27" s="6">
-        <v>18</v>
-      </c>
-      <c r="P27" s="6">
-        <v>8</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>46</v>
-      </c>
-      <c r="R27" s="6">
-        <v>29</v>
-      </c>
-      <c r="S27" s="6">
-        <v>32</v>
-      </c>
-      <c r="T27" s="6">
-        <v>40</v>
-      </c>
-      <c r="U27" s="6">
-        <v>62</v>
-      </c>
-      <c r="V27" s="6">
-        <v>76</v>
-      </c>
-      <c r="W27" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D28" s="6">
-        <v>20</v>
-      </c>
-      <c r="E28" s="6">
-        <v>69</v>
-      </c>
-      <c r="F28" s="6">
-        <v>36</v>
-      </c>
-      <c r="G28" s="6">
-        <v>41</v>
-      </c>
-      <c r="H28" s="6">
-        <v>72</v>
-      </c>
-      <c r="I28" s="6">
-        <v>30</v>
-      </c>
-      <c r="J28" s="6">
-        <v>23</v>
-      </c>
-      <c r="K28" s="6">
-        <v>88</v>
-      </c>
-      <c r="L28" s="6">
-        <v>34</v>
-      </c>
-      <c r="M28" s="6">
-        <v>62</v>
-      </c>
-      <c r="N28" s="6">
-        <v>99</v>
-      </c>
-      <c r="O28" s="6">
-        <v>69</v>
-      </c>
-      <c r="P28" s="6">
-        <v>82</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>67</v>
-      </c>
-      <c r="R28" s="6">
-        <v>59</v>
-      </c>
-      <c r="S28" s="6">
-        <v>85</v>
-      </c>
-      <c r="T28" s="6">
-        <v>74</v>
-      </c>
-      <c r="U28" s="6">
-        <v>4</v>
-      </c>
-      <c r="V28" s="6">
-        <v>36</v>
-      </c>
-      <c r="W28" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D29" s="6">
-        <v>20</v>
-      </c>
-      <c r="E29" s="6">
-        <v>73</v>
-      </c>
-      <c r="F29" s="6">
-        <v>35</v>
-      </c>
-      <c r="G29" s="6">
-        <v>29</v>
-      </c>
-      <c r="H29" s="6">
-        <v>78</v>
-      </c>
-      <c r="I29" s="6">
-        <v>31</v>
-      </c>
-      <c r="J29" s="6">
-        <v>90</v>
-      </c>
-      <c r="K29" s="6">
-        <v>1</v>
-      </c>
-      <c r="L29" s="6">
-        <v>74</v>
-      </c>
-      <c r="M29" s="6">
-        <v>31</v>
-      </c>
-      <c r="N29" s="6">
-        <v>49</v>
-      </c>
-      <c r="O29" s="6">
-        <v>71</v>
-      </c>
-      <c r="P29" s="6">
-        <v>48</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>86</v>
-      </c>
-      <c r="R29" s="6">
-        <v>81</v>
-      </c>
-      <c r="S29" s="6">
-        <v>16</v>
-      </c>
-      <c r="T29" s="6">
-        <v>23</v>
-      </c>
-      <c r="U29" s="6">
-        <v>57</v>
-      </c>
-      <c r="V29" s="6">
-        <v>5</v>
-      </c>
-      <c r="W29" s="6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6">
-        <v>70</v>
-      </c>
-      <c r="F30" s="6">
-        <v>54</v>
-      </c>
-      <c r="G30" s="6">
-        <v>71</v>
-      </c>
-      <c r="H30" s="6">
-        <v>83</v>
-      </c>
-      <c r="I30" s="6">
-        <v>51</v>
-      </c>
-      <c r="J30" s="6">
-        <v>54</v>
-      </c>
-      <c r="K30" s="6">
-        <v>69</v>
-      </c>
-      <c r="L30" s="6">
-        <v>16</v>
-      </c>
-      <c r="M30" s="6">
-        <v>92</v>
-      </c>
-      <c r="N30" s="6">
-        <v>33</v>
-      </c>
-      <c r="O30" s="6">
-        <v>48</v>
-      </c>
-      <c r="P30" s="6">
-        <v>61</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>43</v>
-      </c>
-      <c r="R30" s="6">
-        <v>52</v>
-      </c>
-      <c r="S30" s="6">
-        <v>1</v>
-      </c>
-      <c r="T30" s="6">
-        <v>89</v>
-      </c>
-      <c r="U30" s="6">
-        <v>19</v>
-      </c>
-      <c r="V30" s="6">
-        <v>67</v>
-      </c>
-      <c r="W30" s="6">
         <v>48</v>
       </c>
     </row>

</xml_diff>